<commit_message>
Used terms deep and shallow in diagram.
</commit_message>
<xml_diff>
--- a/diagrams/swap_and_legs.xlsx
+++ b/diagrams/swap_and_legs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Training\enterprise-python\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D101F856-AB4E-4DF4-8445-8D7712A8D4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D826A6D-DFAE-41B5-9459-0558517D7D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{1E47582C-70E2-4F44-B477-E6F31E9C6A07}"/>
   </bookViews>
@@ -112,13 +112,13 @@
     <t>Relational Database, SQL (MySQL, Postgres) - Join from leg to trade</t>
   </si>
   <si>
-    <t>Document Database, NoSQL (MongoDB) - Embed list of each leg attribute in its own column</t>
-  </si>
-  <si>
-    <t>Document Database, NoSQL (MongoDB) - Embed list of leg documents in a single column</t>
-  </si>
-  <si>
     <t>Wide Column Database, NoSQL (Cassandra) - One attribute of one leg per column</t>
+  </si>
+  <si>
+    <t>Document Database, NoSQL (MongoDB) - Deep style of embedding (entire leg document list in a single column)</t>
+  </si>
+  <si>
+    <t>Document Database, NoSQL (MongoDB) - Shallow style of embedding (each leg attribute list in its own column)</t>
   </si>
 </sst>
 </file>
@@ -317,14 +317,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,7 +642,7 @@
   <dimension ref="B2:J32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -767,7 +767,7 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
@@ -866,10 +866,10 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="15"/>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="2" t="s">
@@ -884,10 +884,10 @@
       <c r="E21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -928,10 +928,10 @@
       <c r="E24" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -961,7 +961,7 @@
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>

</xml_diff>

<commit_message>
Removed placeholder columns with ellipsis.
</commit_message>
<xml_diff>
--- a/diagrams/swap_and_legs.xlsx
+++ b/diagrams/swap_and_legs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Training\enterprise-python\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D826A6D-DFAE-41B5-9459-0558517D7D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99362E2F-52FE-463F-BB0C-8E9A2C8B33F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{1E47582C-70E2-4F44-B477-E6F31E9C6A07}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
   <si>
     <t>trade_id</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>L22</t>
-  </si>
-  <si>
-    <t>…</t>
   </si>
   <si>
     <t>trade_type</t>
@@ -302,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -312,7 +309,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -639,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01074092-0384-46DF-97C0-73D41A91A4CA}">
-  <dimension ref="B2:J32"/>
+  <dimension ref="B2:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -652,396 +648,328 @@
     <col min="14" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="4" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="4" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="6" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="G7" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="H7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G8" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="12" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="12" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+        <v>8</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="20" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="20" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+        <v>8</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="D22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="D23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="E24" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="D25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="D26" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="30" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="30" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B30" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="F30" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I30" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    </row>
+    <row r="31" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B31" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I31" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    </row>
+    <row r="32" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B32" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added color to indicate the trade to which the data belongs.
</commit_message>
<xml_diff>
--- a/diagrams/swap_and_legs.xlsx
+++ b/diagrams/swap_and_legs.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Training\enterprise-python\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99362E2F-52FE-463F-BB0C-8E9A2C8B33F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD819B0C-E057-435A-9F9D-6DDB1687BA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{1E47582C-70E2-4F44-B477-E6F31E9C6A07}"/>
   </bookViews>
   <sheets>
-    <sheet name="Swap Schema" sheetId="1" r:id="rId1"/>
+    <sheet name="Swap and Legs Schema" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="29">
   <si>
     <t>trade_id</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Fixed</t>
   </si>
   <si>
-    <t>legs</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
@@ -116,6 +113,15 @@
   </si>
   <si>
     <t>Document Database, NoSQL (MongoDB) - Shallow style of embedding (each leg attribute list in its own column)</t>
+  </si>
+  <si>
+    <t>leg_type[]</t>
+  </si>
+  <si>
+    <t>leg_ccy[]</t>
+  </si>
+  <si>
+    <t>legs[]</t>
   </si>
 </sst>
 </file>
@@ -139,13 +145,25 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -299,28 +317,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,9 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01074092-0384-46DF-97C0-73D41A91A4CA}">
   <dimension ref="B2:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -649,322 +675,322 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="4" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="5" t="s">
+    <row r="8" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="E7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="E8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="6" t="s">
-        <v>26</v>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="12" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
+    <row r="16" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="6" t="s">
-        <v>25</v>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="20" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="11" t="s">
+    </row>
+    <row r="23" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="26" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="10" t="s">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>15</v>
+      <c r="E26" s="19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" s="6" t="s">
-        <v>24</v>
+      <c r="B28" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="30" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="G30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="7" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="31" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="32" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>15</v>
+      <c r="F32" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>